<commit_message>
fix bug for template
</commit_message>
<xml_diff>
--- a/public/template_kategori.xlsx
+++ b/public/template_kategori.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\POS\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E48E9A1D-EFF7-458E-AB62-1334BD6E6211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED437029-DC87-44C3-BB24-37F732738DBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2928" yWindow="2928" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2652" yWindow="2652" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -313,10 +313,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -357,14 +357,6 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>